<commit_message>
Added several new files including main method, see readme
</commit_message>
<xml_diff>
--- a/testing_status.xlsx
+++ b/testing_status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="14370" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="14370" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Function</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Tests writen</t>
+  </si>
+  <si>
+    <t>Indentation not working</t>
   </si>
 </sst>
 </file>
@@ -795,8 +798,8 @@
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="5:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E2" s="21" t="s">
         <v>0</v>
       </c>
@@ -807,102 +810,105 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="8"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>